<commit_message>
mixlog code isolated from bgl, opensetv11 predicted some success
</commit_message>
<xml_diff>
--- a/oclog/BGL/mytest.xlsx
+++ b/oclog/BGL/mytest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="102">
   <si>
     <t>Unnamed: 0.4</t>
   </si>
@@ -127,6 +127,18 @@
     <t>total_oc_time</t>
   </si>
   <si>
+    <t>embedding_size</t>
+  </si>
+  <si>
+    <t>centroid_class_color</t>
+  </si>
+  <si>
+    <t>manual_color_map</t>
+  </si>
+  <si>
+    <t>centroid_black</t>
+  </si>
+  <si>
     <t>2022-04-30_13_50_00.194963_53e9b7c4c85e11ecaed9ac8247733f47</t>
   </si>
   <si>
@@ -145,6 +157,48 @@
     <t>2022-04-30_16_03_30.948726_fab1bca5c87011ec801bac8247733f47</t>
   </si>
   <si>
+    <t>2022-05-01_06_37_19.455265_0c84f550c8eb11ec801bac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_06_43_15.664562_e0d62ef9c8eb11ec9e08ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_07_09_43.525786_9346940ac8ef11ec801bac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_07_57_31.404170_40aa1769c8f611ecb16fac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_08_15_09.536588_b75c48fcc8f811ecaf5eac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_09_53_00.129337_6281a63ac90611ec801bac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_10_08_03.872791_7d2df4e8c90811ecb63aac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_10_28_18.240033_50ffb150c90b11ec9068ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_11_15_45.421261_f20d1209c91111ec8e58ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_11_51_51.291537_fd02a5afc91611ec9be7ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_12_10_08.849765_8b34bdf7c91911ec927aac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_12_20_54.425829_0bffd4f4c91b11ec8927ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_12_32_02.200180_9a061c8ec91c11ec9c76ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-05-01_12_55_36.379416_e4f0bcf4c91f11ecaaa3ac8247733f47</t>
+  </si>
+  <si>
     <t>adam</t>
   </si>
   <si>
@@ -163,6 +217,42 @@
     <t>3.0299346,3.0356452,3.0902934,3.0109043,3.091632,3.0749729</t>
   </si>
   <si>
+    <t>4.2147183,4.20224,4.2091427</t>
+  </si>
+  <si>
+    <t>4.225795,4.262181,4.2305355</t>
+  </si>
+  <si>
+    <t>6.9317627,6.9686093,6.9369645</t>
+  </si>
+  <si>
+    <t>4.225749,4.2621536,4.230554</t>
+  </si>
+  <si>
+    <t>5.8863473,5.9228034,5.8911915</t>
+  </si>
+  <si>
+    <t>7.1860385,7.222196,7.190782</t>
+  </si>
+  <si>
+    <t>8.584136,8.621342,8.589714</t>
+  </si>
+  <si>
+    <t>5.1101565,5.1465626,5.114935</t>
+  </si>
+  <si>
+    <t>7.1757007,7.184386,7.1703844</t>
+  </si>
+  <si>
+    <t>8.485534,8.521918,8.490291</t>
+  </si>
+  <si>
+    <t>8.338195,8.374665,8.343043</t>
+  </si>
+  <si>
+    <t>9.556441,9.562168,9.616707</t>
+  </si>
+  <si>
     <t>ptmodel</t>
   </si>
   <si>
@@ -185,6 +275,48 @@
   </si>
   <si>
     <t>data\ptmodel_2022-04-30_15_54_04.621193/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_06_32_54.674498/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_06_38_51.458644/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_07_05_21.530000/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_07_30_02.847265/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_08_10_47.070988/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_09_48_38.487791/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_09_58_33.602994/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_10_18_43.787556/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_10_28_46.638320/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_11_47_12.648366/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_12_00_32.151000/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_12_11_24.959058/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_12_22_30.992935/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-05-01_12_35_40.835884/</t>
   </si>
   <si>
     <t>train_data</t>
@@ -545,13 +677,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:AP21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:42">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,8 +795,20 @@
       <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:42">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -681,25 +825,25 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H2">
         <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="J2">
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="M2">
         <v>945.9614868164062</v>
@@ -714,10 +858,10 @@
         <v>5</v>
       </c>
       <c r="Q2" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="R2" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="S2" t="b">
         <v>1</v>
@@ -726,13 +870,13 @@
         <v>3</v>
       </c>
       <c r="U2" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="V2">
         <v>192.4874160289764</v>
       </c>
       <c r="W2" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="X2">
         <v>13.9194</v>
@@ -777,7 +921,7 @@
         <v>593.8424024581909</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:42">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -793,23 +937,26 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="J3">
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="M3">
         <v>945.9578857421875</v>
@@ -824,10 +971,10 @@
         <v>5</v>
       </c>
       <c r="Q3" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="R3" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="S3" t="b">
         <v>1</v>
@@ -836,13 +983,13 @@
         <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="V3">
         <v>191.4216840267181</v>
       </c>
       <c r="W3" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="X3">
         <v>14.0725</v>
@@ -887,7 +1034,7 @@
         <v>2496.334201812744</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:42">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -898,25 +1045,31 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="J4">
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="M4">
         <v>613.926025390625</v>
@@ -931,10 +1084,10 @@
         <v>5</v>
       </c>
       <c r="Q4" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="R4" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="S4" t="b">
         <v>1</v>
@@ -943,13 +1096,13 @@
         <v>3</v>
       </c>
       <c r="U4" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="V4">
         <v>184.3464825153351</v>
       </c>
       <c r="W4" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="X4">
         <v>1.7616</v>
@@ -994,7 +1147,7 @@
         <v>565.4998919963837</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:42">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1002,25 +1155,34 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H5">
         <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="J5">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="M5">
         <v>547.7702026367188</v>
@@ -1035,10 +1197,10 @@
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="R5" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="S5" t="b">
         <v>1</v>
@@ -1047,13 +1209,13 @@
         <v>3</v>
       </c>
       <c r="U5" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="V5">
         <v>37.91154718399048</v>
       </c>
       <c r="W5" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="X5">
         <v>12.3821</v>
@@ -1098,30 +1260,42 @@
         <v>177.2827804088593</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:42">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H6">
         <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="J6">
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="M6">
         <v>613.926025390625</v>
@@ -1136,10 +1310,10 @@
         <v>5</v>
       </c>
       <c r="Q6" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="R6" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="S6" t="b">
         <v>1</v>
@@ -1148,13 +1322,13 @@
         <v>3</v>
       </c>
       <c r="U6" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="V6">
         <v>186.1220259666443</v>
       </c>
       <c r="W6" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="X6">
         <v>8.2698</v>
@@ -1199,27 +1373,42 @@
         <v>566.7014346122742</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:42">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H7">
         <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="J7">
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="M7">
         <v>613.926025390625</v>
@@ -1234,10 +1423,10 @@
         <v>5</v>
       </c>
       <c r="Q7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="R7" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="S7" t="b">
         <v>1</v>
@@ -1246,13 +1435,13 @@
         <v>3</v>
       </c>
       <c r="U7" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="V7">
         <v>186.6121981143951</v>
       </c>
       <c r="W7" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="X7">
         <v>8.2698</v>
@@ -1295,6 +1484,1576 @@
       </c>
       <c r="AL7">
         <v>568.2171151638031</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8">
+        <v>220.0150756835938</v>
+      </c>
+      <c r="N8">
+        <v>0.7308999166383123</v>
+      </c>
+      <c r="O8">
+        <v>0.4663073160242972</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>79</v>
+      </c>
+      <c r="R8" t="s">
+        <v>80</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8" t="s">
+        <v>87</v>
+      </c>
+      <c r="V8">
+        <v>75.82041382789612</v>
+      </c>
+      <c r="W8" t="s">
+        <v>101</v>
+      </c>
+      <c r="X8">
+        <v>46.734</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0.3516571969696969</v>
+      </c>
+      <c r="AA8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0.4635416666666667</v>
+      </c>
+      <c r="AC8">
+        <v>46.35</v>
+      </c>
+      <c r="AD8">
+        <v>3</v>
+      </c>
+      <c r="AE8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>5</v>
+      </c>
+      <c r="AG8">
+        <v>3</v>
+      </c>
+      <c r="AH8">
+        <v>2</v>
+      </c>
+      <c r="AJ8">
+        <v>257.1655254364014</v>
+      </c>
+      <c r="AK8">
+        <v>1651367239.455266</v>
+      </c>
+      <c r="AL8">
+        <v>265.8063902854919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9">
+        <v>195.5811004638672</v>
+      </c>
+      <c r="N9">
+        <v>0.7436503704852386</v>
+      </c>
+      <c r="O9">
+        <v>0.5482932316118936</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>79</v>
+      </c>
+      <c r="R9" t="s">
+        <v>80</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9" t="s">
+        <v>88</v>
+      </c>
+      <c r="V9">
+        <v>74.56402206420898</v>
+      </c>
+      <c r="W9" t="s">
+        <v>101</v>
+      </c>
+      <c r="X9">
+        <v>49.8695</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0.3727290034812881</v>
+      </c>
+      <c r="AA9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0.4973958333333333</v>
+      </c>
+      <c r="AC9">
+        <v>49.74</v>
+      </c>
+      <c r="AD9">
+        <v>9</v>
+      </c>
+      <c r="AE9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>5</v>
+      </c>
+      <c r="AG9">
+        <v>3</v>
+      </c>
+      <c r="AH9">
+        <v>2</v>
+      </c>
+      <c r="AJ9">
+        <v>256.6261096000671</v>
+      </c>
+      <c r="AK9">
+        <v>1651367595.665563</v>
+      </c>
+      <c r="AL9">
+        <v>265.2572958469391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10">
+        <v>220.0150756835938</v>
+      </c>
+      <c r="N10">
+        <v>0.8168794658243691</v>
+      </c>
+      <c r="O10">
+        <v>0.5996264043433855</v>
+      </c>
+      <c r="P10">
+        <v>5</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>79</v>
+      </c>
+      <c r="R10" t="s">
+        <v>80</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>3</v>
+      </c>
+      <c r="U10" t="s">
+        <v>89</v>
+      </c>
+      <c r="V10">
+        <v>74.24005770683289</v>
+      </c>
+      <c r="W10" t="s">
+        <v>101</v>
+      </c>
+      <c r="X10">
+        <v>41.7303</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0.4177588827532352</v>
+      </c>
+      <c r="AA10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="AC10">
+        <v>45.83</v>
+      </c>
+      <c r="AD10">
+        <v>7</v>
+      </c>
+      <c r="AE10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>5</v>
+      </c>
+      <c r="AG10">
+        <v>3</v>
+      </c>
+      <c r="AH10">
+        <v>2</v>
+      </c>
+      <c r="AJ10">
+        <v>254.4074232578278</v>
+      </c>
+      <c r="AK10">
+        <v>1651369183.525787</v>
+      </c>
+      <c r="AL10">
+        <v>262.9977917671204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11">
+        <v>195.5748901367188</v>
+      </c>
+      <c r="N11">
+        <v>0.9296564248375482</v>
+      </c>
+      <c r="O11">
+        <v>0.6753382268278642</v>
+      </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>79</v>
+      </c>
+      <c r="R11" t="s">
+        <v>80</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>3</v>
+      </c>
+      <c r="U11" t="s">
+        <v>90</v>
+      </c>
+      <c r="V11">
+        <v>73.96717047691345</v>
+      </c>
+      <c r="W11" t="s">
+        <v>101</v>
+      </c>
+      <c r="X11">
+        <v>42.4812</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0.4229910714285715</v>
+      </c>
+      <c r="AA11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0.4921875</v>
+      </c>
+      <c r="AC11">
+        <v>49.22</v>
+      </c>
+      <c r="AD11">
+        <v>7</v>
+      </c>
+      <c r="AE11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>50</v>
+      </c>
+      <c r="AG11">
+        <v>3</v>
+      </c>
+      <c r="AH11">
+        <v>2</v>
+      </c>
+      <c r="AJ11">
+        <v>1641.06181883812</v>
+      </c>
+      <c r="AK11">
+        <v>1651372051.404171</v>
+      </c>
+      <c r="AL11">
+        <v>1649.61891579628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12">
+        <v>200.7127380371094</v>
+      </c>
+      <c r="N12">
+        <v>0.818777674199278</v>
+      </c>
+      <c r="O12">
+        <v>0.5128917378917379</v>
+      </c>
+      <c r="P12">
+        <v>5</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>79</v>
+      </c>
+      <c r="R12" t="s">
+        <v>80</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
+      <c r="U12" t="s">
+        <v>91</v>
+      </c>
+      <c r="V12">
+        <v>74.55869770050049</v>
+      </c>
+      <c r="W12" t="s">
+        <v>101</v>
+      </c>
+      <c r="X12">
+        <v>28.5728</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0.2815890325626025</v>
+      </c>
+      <c r="AA12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0.3125</v>
+      </c>
+      <c r="AC12">
+        <v>31.25</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+      <c r="AE12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF12">
+        <v>5</v>
+      </c>
+      <c r="AG12">
+        <v>3</v>
+      </c>
+      <c r="AH12">
+        <v>2</v>
+      </c>
+      <c r="AJ12">
+        <v>255.0124139785767</v>
+      </c>
+      <c r="AK12">
+        <v>1651373109.536588</v>
+      </c>
+      <c r="AL12">
+        <v>263.6070122718811</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13">
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13">
+        <v>220.0150756835938</v>
+      </c>
+      <c r="N13">
+        <v>0.8168794658243691</v>
+      </c>
+      <c r="O13">
+        <v>0.5996264043433855</v>
+      </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>79</v>
+      </c>
+      <c r="R13" t="s">
+        <v>80</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>3</v>
+      </c>
+      <c r="U13" t="s">
+        <v>92</v>
+      </c>
+      <c r="V13">
+        <v>74.48916435241699</v>
+      </c>
+      <c r="W13" t="s">
+        <v>101</v>
+      </c>
+      <c r="X13">
+        <v>55.6403</v>
+      </c>
+      <c r="Y13">
+        <v>27.3859</v>
+      </c>
+      <c r="Z13">
+        <v>0.4847972644959738</v>
+      </c>
+      <c r="AA13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0.5442708333333334</v>
+      </c>
+      <c r="AC13">
+        <v>54.43</v>
+      </c>
+      <c r="AD13">
+        <v>3</v>
+      </c>
+      <c r="AE13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <v>5</v>
+      </c>
+      <c r="AG13">
+        <v>3</v>
+      </c>
+      <c r="AH13">
+        <v>2</v>
+      </c>
+      <c r="AJ13">
+        <v>253.9911785125732</v>
+      </c>
+      <c r="AK13">
+        <v>1651378980.129337</v>
+      </c>
+      <c r="AL13">
+        <v>262.6715466976166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14">
+        <v>50</v>
+      </c>
+      <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M14">
+        <v>195.5696411132812</v>
+      </c>
+      <c r="N14">
+        <v>0.8844412986907203</v>
+      </c>
+      <c r="O14">
+        <v>0.6718659104130309</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>79</v>
+      </c>
+      <c r="R14" t="s">
+        <v>80</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="U14" t="s">
+        <v>93</v>
+      </c>
+      <c r="V14">
+        <v>75.48118042945862</v>
+      </c>
+      <c r="W14" t="s">
+        <v>101</v>
+      </c>
+      <c r="X14">
+        <v>56.6416</v>
+      </c>
+      <c r="Y14">
+        <v>16.9014</v>
+      </c>
+      <c r="Z14">
+        <v>0.4652445925553321</v>
+      </c>
+      <c r="AA14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0.5390625</v>
+      </c>
+      <c r="AC14">
+        <v>53.91</v>
+      </c>
+      <c r="AD14">
+        <v>3</v>
+      </c>
+      <c r="AE14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <v>15</v>
+      </c>
+      <c r="AG14">
+        <v>3</v>
+      </c>
+      <c r="AH14">
+        <v>2</v>
+      </c>
+      <c r="AJ14">
+        <v>562.8246974945068</v>
+      </c>
+      <c r="AK14">
+        <v>1651379883.873793</v>
+      </c>
+      <c r="AL14">
+        <v>571.3394181728363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" t="s">
+        <v>72</v>
+      </c>
+      <c r="M15">
+        <v>277.5717163085938</v>
+      </c>
+      <c r="N15">
+        <v>0.8441249837852606</v>
+      </c>
+      <c r="O15">
+        <v>0.6718661872532431</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>79</v>
+      </c>
+      <c r="R15" t="s">
+        <v>80</v>
+      </c>
+      <c r="S15" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+      <c r="U15" t="s">
+        <v>94</v>
+      </c>
+      <c r="V15">
+        <v>76.27985858917236</v>
+      </c>
+      <c r="W15" t="s">
+        <v>101</v>
+      </c>
+      <c r="X15">
+        <v>56.3817</v>
+      </c>
+      <c r="Y15">
+        <v>15.0235</v>
+      </c>
+      <c r="Z15">
+        <v>0.453803391393383</v>
+      </c>
+      <c r="AA15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0.5286458333333334</v>
+      </c>
+      <c r="AC15">
+        <v>52.86</v>
+      </c>
+      <c r="AD15">
+        <v>3</v>
+      </c>
+      <c r="AE15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>15</v>
+      </c>
+      <c r="AG15">
+        <v>3</v>
+      </c>
+      <c r="AH15">
+        <v>2.5</v>
+      </c>
+      <c r="AJ15">
+        <v>566.7858638763428</v>
+      </c>
+      <c r="AK15">
+        <v>1651381098.240034</v>
+      </c>
+      <c r="AL15">
+        <v>575.5970702171326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L16" t="s">
+        <v>73</v>
+      </c>
+      <c r="M16">
+        <v>237.5995330810547</v>
+      </c>
+      <c r="N16">
+        <v>0.9545454545454546</v>
+      </c>
+      <c r="O16">
+        <v>0.6840277777777778</v>
+      </c>
+      <c r="P16">
+        <v>16</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>79</v>
+      </c>
+      <c r="R16" t="s">
+        <v>80</v>
+      </c>
+      <c r="S16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
+      <c r="U16" t="s">
+        <v>95</v>
+      </c>
+      <c r="V16">
+        <v>75.79198145866394</v>
+      </c>
+      <c r="W16" t="s">
+        <v>101</v>
+      </c>
+      <c r="X16">
+        <v>56.5217</v>
+      </c>
+      <c r="Y16">
+        <v>12.5</v>
+      </c>
+      <c r="Z16">
+        <v>0.4476760643115942</v>
+      </c>
+      <c r="AA16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0.5260416666666666</v>
+      </c>
+      <c r="AC16">
+        <v>52.6</v>
+      </c>
+      <c r="AD16">
+        <v>3</v>
+      </c>
+      <c r="AE16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF16">
+        <v>100</v>
+      </c>
+      <c r="AG16">
+        <v>8</v>
+      </c>
+      <c r="AH16">
+        <v>2.5</v>
+      </c>
+      <c r="AJ16">
+        <v>2811.343915462494</v>
+      </c>
+      <c r="AK16">
+        <v>1651383945.422262</v>
+      </c>
+      <c r="AL16">
+        <v>2819.777952194214</v>
+      </c>
+      <c r="AM16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17">
+        <v>285.7010803222656</v>
+      </c>
+      <c r="N17">
+        <v>0.7939375544218139</v>
+      </c>
+      <c r="O17">
+        <v>0.6805201247165533</v>
+      </c>
+      <c r="P17">
+        <v>16</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>79</v>
+      </c>
+      <c r="R17" t="s">
+        <v>80</v>
+      </c>
+      <c r="S17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+      <c r="U17" t="s">
+        <v>96</v>
+      </c>
+      <c r="V17">
+        <v>91.77626776695251</v>
+      </c>
+      <c r="W17" t="s">
+        <v>101</v>
+      </c>
+      <c r="X17">
+        <v>59.5537</v>
+      </c>
+      <c r="Y17">
+        <v>39.834</v>
+      </c>
+      <c r="Z17">
+        <v>0.5488681715394365</v>
+      </c>
+      <c r="AA17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0.6223958333333334</v>
+      </c>
+      <c r="AC17">
+        <v>62.24</v>
+      </c>
+      <c r="AD17">
+        <v>3</v>
+      </c>
+      <c r="AE17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF17">
+        <v>5</v>
+      </c>
+      <c r="AG17">
+        <v>8</v>
+      </c>
+      <c r="AH17">
+        <v>2.5</v>
+      </c>
+      <c r="AJ17">
+        <v>271.0493175983429</v>
+      </c>
+      <c r="AK17">
+        <v>1651386111.292539</v>
+      </c>
+      <c r="AL17">
+        <v>279.6347074508667</v>
+      </c>
+      <c r="AM17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18">
+        <v>50</v>
+      </c>
+      <c r="I18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18">
+        <v>275.6136779785156</v>
+      </c>
+      <c r="N18">
+        <v>0.8160362107985774</v>
+      </c>
+      <c r="O18">
+        <v>0.6805555555555556</v>
+      </c>
+      <c r="P18">
+        <v>16</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>79</v>
+      </c>
+      <c r="R18" t="s">
+        <v>80</v>
+      </c>
+      <c r="S18" t="b">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>3</v>
+      </c>
+      <c r="U18" t="s">
+        <v>97</v>
+      </c>
+      <c r="V18">
+        <v>73.94604325294495</v>
+      </c>
+      <c r="W18" t="s">
+        <v>101</v>
+      </c>
+      <c r="X18">
+        <v>56.691</v>
+      </c>
+      <c r="Y18">
+        <v>12.6214</v>
+      </c>
+      <c r="Z18">
+        <v>0.4538030319136371</v>
+      </c>
+      <c r="AA18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0.53125</v>
+      </c>
+      <c r="AC18">
+        <v>53.12</v>
+      </c>
+      <c r="AD18">
+        <v>3</v>
+      </c>
+      <c r="AE18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF18">
+        <v>15</v>
+      </c>
+      <c r="AG18">
+        <v>8</v>
+      </c>
+      <c r="AH18">
+        <v>2.5</v>
+      </c>
+      <c r="AJ18">
+        <v>569.1148836612701</v>
+      </c>
+      <c r="AK18">
+        <v>1651387208.850764</v>
+      </c>
+      <c r="AL18">
+        <v>577.7068881988525</v>
+      </c>
+      <c r="AM18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19">
+        <v>241.3980865478516</v>
+      </c>
+      <c r="N19">
+        <v>0.8925087683579151</v>
+      </c>
+      <c r="O19">
+        <v>0.6753382268278642</v>
+      </c>
+      <c r="P19">
+        <v>16</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>79</v>
+      </c>
+      <c r="R19" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" t="b">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+      <c r="U19" t="s">
+        <v>98</v>
+      </c>
+      <c r="V19">
+        <v>73.57297420501709</v>
+      </c>
+      <c r="W19" t="s">
+        <v>101</v>
+      </c>
+      <c r="X19">
+        <v>56.1275</v>
+      </c>
+      <c r="Y19">
+        <v>13.3333</v>
+      </c>
+      <c r="Z19">
+        <v>0.4491651348039216</v>
+      </c>
+      <c r="AA19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0.5260416666666666</v>
+      </c>
+      <c r="AC19">
+        <v>52.6</v>
+      </c>
+      <c r="AD19">
+        <v>3</v>
+      </c>
+      <c r="AE19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>15</v>
+      </c>
+      <c r="AG19">
+        <v>8</v>
+      </c>
+      <c r="AH19">
+        <v>3</v>
+      </c>
+      <c r="AJ19">
+        <v>561.8725116252899</v>
+      </c>
+      <c r="AK19">
+        <v>1651387854.425829</v>
+      </c>
+      <c r="AL19">
+        <v>570.4632661342621</v>
+      </c>
+      <c r="AM19">
+        <v>22</v>
+      </c>
+      <c r="AN19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20" t="s">
+        <v>77</v>
+      </c>
+      <c r="M20">
+        <v>217.0464019775391</v>
+      </c>
+      <c r="N20">
+        <v>0.958647224832341</v>
+      </c>
+      <c r="O20">
+        <v>0.6788104490500864</v>
+      </c>
+      <c r="P20">
+        <v>16</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>79</v>
+      </c>
+      <c r="R20" t="s">
+        <v>80</v>
+      </c>
+      <c r="S20" t="b">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
+      <c r="U20" t="s">
+        <v>99</v>
+      </c>
+      <c r="V20">
+        <v>74.2982120513916</v>
+      </c>
+      <c r="W20" t="s">
+        <v>101</v>
+      </c>
+      <c r="X20">
+        <v>57.1252</v>
+      </c>
+      <c r="Y20">
+        <v>17.1429</v>
+      </c>
+      <c r="Z20">
+        <v>0.4736739909718535</v>
+      </c>
+      <c r="AA20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0.546875</v>
+      </c>
+      <c r="AC20">
+        <v>54.69</v>
+      </c>
+      <c r="AD20">
+        <v>3</v>
+      </c>
+      <c r="AE20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF20">
+        <v>15</v>
+      </c>
+      <c r="AG20">
+        <v>8</v>
+      </c>
+      <c r="AH20">
+        <v>3</v>
+      </c>
+      <c r="AJ20">
+        <v>563.5545132160187</v>
+      </c>
+      <c r="AK20">
+        <v>1651388522.200181</v>
+      </c>
+      <c r="AL20">
+        <v>572.1595890522003</v>
+      </c>
+      <c r="AM20">
+        <v>22</v>
+      </c>
+      <c r="AO20">
+        <v>1</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <v>50</v>
+      </c>
+      <c r="I21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L21" t="s">
+        <v>78</v>
+      </c>
+      <c r="M21">
+        <v>479.0527648925781</v>
+      </c>
+      <c r="N21">
+        <v>0.92913982569155</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>16</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>79</v>
+      </c>
+      <c r="R21" t="s">
+        <v>80</v>
+      </c>
+      <c r="S21" t="b">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>3</v>
+      </c>
+      <c r="U21" t="s">
+        <v>100</v>
+      </c>
+      <c r="V21">
+        <v>148.8147990703583</v>
+      </c>
+      <c r="W21" t="s">
+        <v>101</v>
+      </c>
+      <c r="X21">
+        <v>88.88890000000001</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0.6666666666666665</v>
+      </c>
+      <c r="AA21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0.75</v>
+      </c>
+      <c r="AC21">
+        <v>75</v>
+      </c>
+      <c r="AD21">
+        <v>3</v>
+      </c>
+      <c r="AE21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF21">
+        <v>15</v>
+      </c>
+      <c r="AG21">
+        <v>8</v>
+      </c>
+      <c r="AH21">
+        <v>3</v>
+      </c>
+      <c r="AJ21">
+        <v>1179.359867811203</v>
+      </c>
+      <c r="AK21">
+        <v>1651389936.380416</v>
+      </c>
+      <c r="AL21">
+        <v>1198.463131189346</v>
+      </c>
+      <c r="AM21">
+        <v>22</v>
+      </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>